<commit_message>
update lmb model multiple compars, and effects
</commit_message>
<xml_diff>
--- a/results/accel-glmm-results/habitat-season/lmb/glmm_multi_comp_hab_season_LMB.xlsx
+++ b/results/accel-glmm-results/habitat-season/lmb/glmm_multi_comp_hab_season_LMB.xlsx
@@ -467,10 +467,10 @@
         <v>0</v>
       </c>
       <c r="G2" t="n">
-        <v>0.806894511460617</v>
+        <v>0.806894511527605</v>
       </c>
       <c r="H2" t="n">
-        <v>0.0902626890121446</v>
+        <v>0.0902626890281051</v>
       </c>
       <c r="I2" t="e">
         <v>#NUM!</v>
@@ -479,7 +479,7 @@
         <v>1</v>
       </c>
       <c r="K2" t="n">
-        <v>-1.91805909292759</v>
+        <v>-1.91805909200552</v>
       </c>
       <c r="L2" t="n">
         <v>1</v>
@@ -505,10 +505,10 @@
         <v>0</v>
       </c>
       <c r="G3" t="n">
-        <v>0.645651656549176</v>
+        <v>0.645651656539064</v>
       </c>
       <c r="H3" t="n">
-        <v>0.00917148459720282</v>
+        <v>0.00917148459690653</v>
       </c>
       <c r="I3" t="e">
         <v>#NUM!</v>
@@ -517,7 +517,7 @@
         <v>1</v>
       </c>
       <c r="K3" t="n">
-        <v>-30.7986636860888</v>
+        <v>-30.798663687704</v>
       </c>
       <c r="L3" t="n">
         <v>0</v>
@@ -543,10 +543,10 @@
         <v>0</v>
       </c>
       <c r="G4" t="n">
-        <v>1.04661626773175</v>
+        <v>1.04661626774275</v>
       </c>
       <c r="H4" t="n">
-        <v>0.0264884636899569</v>
+        <v>0.0264884636905745</v>
       </c>
       <c r="I4" t="e">
         <v>#NUM!</v>
@@ -555,7 +555,7 @@
         <v>1</v>
       </c>
       <c r="K4" t="n">
-        <v>1.800266934792</v>
+        <v>1.80026693518426</v>
       </c>
       <c r="L4" t="n">
         <v>1</v>
@@ -581,10 +581,10 @@
         <v>0</v>
       </c>
       <c r="G5" t="n">
-        <v>0.800168606154522</v>
+        <v>0.80016860607556</v>
       </c>
       <c r="H5" t="n">
-        <v>0.0897055388561325</v>
+        <v>0.0897055388556336</v>
       </c>
       <c r="I5" t="e">
         <v>#NUM!</v>
@@ -593,7 +593,7 @@
         <v>1</v>
       </c>
       <c r="K5" t="n">
-        <v>-1.98854878730234</v>
+        <v>-1.9885487879974</v>
       </c>
       <c r="L5" t="n">
         <v>1</v>
@@ -619,10 +619,10 @@
         <v>0</v>
       </c>
       <c r="G6" t="n">
-        <v>0.77095544598149</v>
+        <v>0.770955446037391</v>
       </c>
       <c r="H6" t="n">
-        <v>0.0878427688068737</v>
+        <v>0.0878427688212459</v>
       </c>
       <c r="I6" t="e">
         <v>#NUM!</v>
@@ -631,7 +631,7 @@
         <v>1</v>
       </c>
       <c r="K6" t="n">
-        <v>-2.28299440588269</v>
+        <v>-2.28299440503832</v>
       </c>
       <c r="L6" t="n">
         <v>1</v>
@@ -657,10 +657,10 @@
         <v>0</v>
       </c>
       <c r="G7" t="n">
-        <v>0.616894344618247</v>
+        <v>0.616894344602101</v>
       </c>
       <c r="H7" t="n">
-        <v>0.0165133081613456</v>
+        <v>0.0165133081610238</v>
       </c>
       <c r="I7" t="e">
         <v>#NUM!</v>
@@ -669,7 +669,7 @@
         <v>1</v>
       </c>
       <c r="K7" t="n">
-        <v>-18.0457751574743</v>
+        <v>-18.0457751583314</v>
       </c>
       <c r="L7" t="n">
         <v>0</v>
@@ -695,10 +695,10 @@
         <v>0</v>
       </c>
       <c r="G8" t="n">
-        <v>0.627433958637207</v>
+        <v>0.627433958602343</v>
       </c>
       <c r="H8" t="n">
-        <v>0.0697424905167372</v>
+        <v>0.0697424905055744</v>
       </c>
       <c r="I8" t="e">
         <v>#NUM!</v>
@@ -707,7 +707,7 @@
         <v>1</v>
       </c>
       <c r="K8" t="n">
-        <v>-4.19339119787546</v>
+        <v>-4.19339119881354</v>
       </c>
       <c r="L8" t="n">
         <v>0.004</v>
@@ -733,10 +733,10 @@
         <v>0</v>
       </c>
       <c r="G9" t="n">
-        <v>0.619592650962479</v>
+        <v>0.619592650944754</v>
       </c>
       <c r="H9" t="n">
-        <v>0.0861829085510776</v>
+        <v>0.0861829085470962</v>
       </c>
       <c r="I9" t="e">
         <v>#NUM!</v>
@@ -745,7 +745,7 @@
         <v>1</v>
       </c>
       <c r="K9" t="n">
-        <v>-3.44145596080156</v>
+        <v>-3.44145596106777</v>
       </c>
       <c r="L9" t="n">
         <v>0.089</v>
@@ -771,10 +771,10 @@
         <v>0</v>
       </c>
       <c r="G10" t="n">
-        <v>0.565783569054377</v>
+        <v>0.565783569050805</v>
       </c>
       <c r="H10" t="n">
-        <v>0.0368048797946356</v>
+        <v>0.0368048797939713</v>
       </c>
       <c r="I10" t="e">
         <v>#NUM!</v>
@@ -783,7 +783,7 @@
         <v>1</v>
       </c>
       <c r="K10" t="n">
-        <v>-8.75531850401898</v>
+        <v>-8.7553185042188</v>
       </c>
       <c r="L10" t="n">
         <v>0</v>
@@ -837,10 +837,10 @@
         <v>0</v>
       </c>
       <c r="G12" t="n">
-        <v>0.767873175690476</v>
+        <v>0.76787317560476</v>
       </c>
       <c r="H12" t="n">
-        <v>0.0961576189688975</v>
+        <v>0.0961576189566994</v>
       </c>
       <c r="I12" t="e">
         <v>#NUM!</v>
@@ -849,7 +849,7 @@
         <v>1</v>
       </c>
       <c r="K12" t="n">
-        <v>-2.10923354763715</v>
+        <v>-2.10923354856069</v>
       </c>
       <c r="L12" t="n">
         <v>1</v>
@@ -875,10 +875,10 @@
         <v>0</v>
       </c>
       <c r="G13" t="n">
-        <v>0.70118653803979</v>
+        <v>0.701186537977149</v>
       </c>
       <c r="H13" t="n">
-        <v>0.0868001359389384</v>
+        <v>0.0868001359379861</v>
       </c>
       <c r="I13" t="e">
         <v>#NUM!</v>
@@ -887,7 +887,7 @@
         <v>1</v>
       </c>
       <c r="K13" t="n">
-        <v>-2.86760064783461</v>
+        <v>-2.86760064833156</v>
       </c>
       <c r="L13" t="n">
         <v>0.633</v>
@@ -913,10 +913,10 @@
         <v>0</v>
       </c>
       <c r="G14" t="n">
-        <v>0.876298485902336</v>
+        <v>0.876298485910526</v>
       </c>
       <c r="H14" t="n">
-        <v>0.0574921183471181</v>
+        <v>0.0574921183469477</v>
       </c>
       <c r="I14" t="e">
         <v>#NUM!</v>
@@ -925,7 +925,7 @@
         <v>1</v>
       </c>
       <c r="K14" t="n">
-        <v>-2.01269168038789</v>
+        <v>-2.01269168027021</v>
       </c>
       <c r="L14" t="n">
         <v>1</v>
@@ -951,10 +951,10 @@
         <v>0</v>
       </c>
       <c r="G15" t="n">
-        <v>0.591996006621674</v>
+        <v>0.591996006598516</v>
       </c>
       <c r="H15" t="n">
-        <v>0.083334690143336</v>
+        <v>0.0833346901386825</v>
       </c>
       <c r="I15" t="e">
         <v>#NUM!</v>
@@ -963,7 +963,7 @@
         <v>1</v>
       </c>
       <c r="K15" t="n">
-        <v>-3.72422452899222</v>
+        <v>-3.72422452933239</v>
       </c>
       <c r="L15" t="n">
         <v>0.03</v>
@@ -989,10 +989,10 @@
         <v>0</v>
       </c>
       <c r="G16" t="n">
-        <v>0.540583580150683</v>
+        <v>0.540583580141587</v>
       </c>
       <c r="H16" t="n">
-        <v>0.0370153184702524</v>
+        <v>0.0370153184693067</v>
       </c>
       <c r="I16" t="e">
         <v>#NUM!</v>
@@ -1001,7 +1001,7 @@
         <v>1</v>
       </c>
       <c r="K16" t="n">
-        <v>-8.98320553908886</v>
+        <v>-8.98320553941296</v>
       </c>
       <c r="L16" t="n">
         <v>0</v>
@@ -1055,10 +1055,10 @@
         <v>0</v>
       </c>
       <c r="G18" t="n">
-        <v>0.416571024892887</v>
+        <v>0.416571024803953</v>
       </c>
       <c r="H18" t="n">
-        <v>0.0715404104045065</v>
+        <v>0.0715404103555121</v>
       </c>
       <c r="I18" t="e">
         <v>#NUM!</v>
@@ -1067,7 +1067,7 @@
         <v>1</v>
       </c>
       <c r="K18" t="n">
-        <v>-5.09908369150672</v>
+        <v>-5.09908369515335</v>
       </c>
       <c r="L18" t="n">
         <v>0</v>
@@ -1093,10 +1093,10 @@
         <v>0</v>
       </c>
       <c r="G19" t="n">
-        <v>0.687969926417134</v>
+        <v>0.68796992637866</v>
       </c>
       <c r="H19" t="n">
-        <v>0.0939617477633459</v>
+        <v>0.0939617477537928</v>
       </c>
       <c r="I19" t="e">
         <v>#NUM!</v>
@@ -1105,7 +1105,7 @@
         <v>1</v>
       </c>
       <c r="K19" t="n">
-        <v>-2.73843073358374</v>
+        <v>-2.73843073411848</v>
       </c>
       <c r="L19" t="n">
         <v>0.945</v>
@@ -1131,10 +1131,10 @@
         <v>0</v>
       </c>
       <c r="G20" t="n">
-        <v>0.479296118484896</v>
+        <v>0.479296118500215</v>
       </c>
       <c r="H20" t="n">
-        <v>0.024617855984561</v>
+        <v>0.024617855986942</v>
       </c>
       <c r="I20" t="e">
         <v>#NUM!</v>
@@ -1143,7 +1143,7 @@
         <v>1</v>
       </c>
       <c r="K20" t="n">
-        <v>-14.3185475654058</v>
+        <v>-14.3185475638563</v>
       </c>
       <c r="L20" t="n">
         <v>0</v>
@@ -1197,10 +1197,10 @@
         <v>0</v>
       </c>
       <c r="G22" t="n">
-        <v>0.852614457832649</v>
+        <v>0.852614457714183</v>
       </c>
       <c r="H22" t="n">
-        <v>0.104371784976554</v>
+        <v>0.10437178495684</v>
       </c>
       <c r="I22" t="e">
         <v>#NUM!</v>
@@ -1209,7 +1209,7 @@
         <v>1</v>
       </c>
       <c r="K22" t="n">
-        <v>-1.30253127756509</v>
+        <v>-1.30253127876518</v>
       </c>
       <c r="L22" t="n">
         <v>1</v>
@@ -1235,10 +1235,10 @@
         <v>0</v>
       </c>
       <c r="G23" t="n">
-        <v>0.59400096502985</v>
+        <v>0.594000964999522</v>
       </c>
       <c r="H23" t="n">
-        <v>0.0632667905556599</v>
+        <v>0.0632667905586196</v>
       </c>
       <c r="I23" t="e">
         <v>#NUM!</v>
@@ -1247,7 +1247,7 @@
         <v>1</v>
       </c>
       <c r="K23" t="n">
-        <v>-4.89039913241678</v>
+        <v>-4.89039913241768</v>
       </c>
       <c r="L23" t="n">
         <v>0</v>
@@ -1273,10 +1273,10 @@
         <v>0</v>
       </c>
       <c r="G24" t="n">
-        <v>0.74234475141998</v>
+        <v>0.742344751455333</v>
       </c>
       <c r="H24" t="n">
-        <v>0.0386208576968557</v>
+        <v>0.0386208577010846</v>
       </c>
       <c r="I24" t="e">
         <v>#NUM!</v>
@@ -1285,7 +1285,7 @@
         <v>1</v>
       </c>
       <c r="K24" t="n">
-        <v>-5.72683612356873</v>
+        <v>-5.72683612229899</v>
       </c>
       <c r="L24" t="n">
         <v>0</v>
@@ -1311,10 +1311,10 @@
         <v>0</v>
       </c>
       <c r="G25" t="n">
-        <v>0.657327759588636</v>
+        <v>0.657327759544966</v>
       </c>
       <c r="H25" t="n">
-        <v>0.0908970509101764</v>
+        <v>0.0908970509001243</v>
       </c>
       <c r="I25" t="e">
         <v>#NUM!</v>
@@ -1323,7 +1323,7 @@
         <v>1</v>
       </c>
       <c r="K25" t="n">
-        <v>-3.03416509599082</v>
+        <v>-3.03416509660521</v>
       </c>
       <c r="L25" t="n">
         <v>0.369</v>
@@ -1349,10 +1349,10 @@
         <v>0</v>
       </c>
       <c r="G26" t="n">
-        <v>0.457948278908023</v>
+        <v>0.457948278917847</v>
       </c>
       <c r="H26" t="n">
-        <v>0.0255002058413214</v>
+        <v>0.0255002058433439</v>
       </c>
       <c r="I26" t="e">
         <v>#NUM!</v>
@@ -1361,7 +1361,7 @@
         <v>1</v>
       </c>
       <c r="K26" t="n">
-        <v>-14.0256578148835</v>
+        <v>-14.0256578136868</v>
       </c>
       <c r="L26" t="n">
         <v>0</v>
@@ -1415,10 +1415,10 @@
         <v>0</v>
       </c>
       <c r="G28" t="n">
-        <v>1.22858971453345</v>
+        <v>1.2285897145194</v>
       </c>
       <c r="H28" t="n">
-        <v>0.112878769326398</v>
+        <v>0.112878769332676</v>
       </c>
       <c r="I28" t="e">
         <v>#NUM!</v>
@@ -1427,7 +1427,7 @@
         <v>1</v>
       </c>
       <c r="K28" t="n">
-        <v>2.24068710279387</v>
+        <v>2.24068710251919</v>
       </c>
       <c r="L28" t="n">
         <v>1</v>
@@ -1453,10 +1453,10 @@
         <v>0</v>
       </c>
       <c r="G29" t="n">
-        <v>0.775173114717797</v>
+        <v>0.775173114703754</v>
       </c>
       <c r="H29" t="n">
-        <v>0.071623715593157</v>
+        <v>0.0716237155964431</v>
       </c>
       <c r="I29" t="e">
         <v>#NUM!</v>
@@ -1465,7 +1465,7 @@
         <v>1</v>
       </c>
       <c r="K29" t="n">
-        <v>-2.75624467924182</v>
+        <v>-2.75624467926151</v>
       </c>
       <c r="L29" t="n">
         <v>0.895</v>
@@ -1491,10 +1491,10 @@
         <v>0</v>
       </c>
       <c r="G30" t="n">
-        <v>0.740326849673318</v>
+        <v>0.740326849672927</v>
       </c>
       <c r="H30" t="n">
-        <v>0.0667623748603438</v>
+        <v>0.0667623748648762</v>
       </c>
       <c r="I30" t="e">
         <v>#NUM!</v>
@@ -1503,7 +1503,7 @@
         <v>1</v>
       </c>
       <c r="K30" t="n">
-        <v>-3.33405250159734</v>
+        <v>-3.33405250137509</v>
       </c>
       <c r="L30" t="n">
         <v>0.131</v>
@@ -1529,10 +1529,10 @@
         <v>0</v>
       </c>
       <c r="G31" t="n">
-        <v>1.48263752894106</v>
+        <v>1.48263752892013</v>
       </c>
       <c r="H31" t="n">
-        <v>0.135002786580929</v>
+        <v>0.135002786588233</v>
       </c>
       <c r="I31" t="e">
         <v>#NUM!</v>
@@ -1541,7 +1541,7 @@
         <v>1</v>
       </c>
       <c r="K31" t="n">
-        <v>4.32506768774099</v>
+        <v>4.32506768729081</v>
       </c>
       <c r="L31" t="n">
         <v>0.002</v>
@@ -1567,10 +1567,10 @@
         <v>0</v>
       </c>
       <c r="G32" t="n">
-        <v>0.960687058478811</v>
+        <v>0.96068705838165</v>
       </c>
       <c r="H32" t="n">
-        <v>0.0721093839526125</v>
+        <v>0.0721093839531676</v>
       </c>
       <c r="I32" t="e">
         <v>#NUM!</v>
@@ -1579,7 +1579,7 @@
         <v>1</v>
       </c>
       <c r="K32" t="n">
-        <v>-0.534325152229902</v>
+        <v>-0.534325153519166</v>
       </c>
       <c r="L32" t="n">
         <v>1</v>
@@ -1605,10 +1605,10 @@
         <v>0</v>
       </c>
       <c r="G33" t="n">
-        <v>0.917501407133381</v>
+        <v>0.917501407056725</v>
       </c>
       <c r="H33" t="n">
-        <v>0.0658778339141142</v>
+        <v>0.0658778339166097</v>
       </c>
       <c r="I33" t="e">
         <v>#NUM!</v>
@@ -1617,7 +1617,7 @@
         <v>1</v>
       </c>
       <c r="K33" t="n">
-        <v>-1.19915813425222</v>
+        <v>-1.19915813527022</v>
       </c>
       <c r="L33" t="n">
         <v>1</v>
@@ -1643,10 +1643,10 @@
         <v>0</v>
       </c>
       <c r="G34" t="n">
-        <v>1.14663509674885</v>
+        <v>1.1466350967662</v>
       </c>
       <c r="H34" t="n">
-        <v>0.103747332853404</v>
+        <v>0.103747332861981</v>
       </c>
       <c r="I34" t="e">
         <v>#NUM!</v>
@@ -1655,7 +1655,7 @@
         <v>1</v>
       </c>
       <c r="K34" t="n">
-        <v>1.51228921667194</v>
+        <v>1.51228921673706</v>
       </c>
       <c r="L34" t="n">
         <v>1</v>
@@ -1681,10 +1681,10 @@
         <v>0</v>
       </c>
       <c r="G35" t="n">
-        <v>0.740646919618178</v>
+        <v>0.740646919596974</v>
       </c>
       <c r="H35" t="n">
-        <v>0.0702877992554738</v>
+        <v>0.0702877992577953</v>
       </c>
       <c r="I35" t="e">
         <v>#NUM!</v>
@@ -1693,7 +1693,7 @@
         <v>1</v>
       </c>
       <c r="K35" t="n">
-        <v>-3.16364090920068</v>
+        <v>-3.16364090930728</v>
       </c>
       <c r="L35" t="n">
         <v>0.238</v>
@@ -1719,10 +1719,10 @@
         <v>0</v>
       </c>
       <c r="G36" t="n">
-        <v>0.707352706525161</v>
+        <v>0.707352706517352</v>
       </c>
       <c r="H36" t="n">
-        <v>0.0656022353781907</v>
+        <v>0.0656022353817783</v>
       </c>
       <c r="I36" t="e">
         <v>#NUM!</v>
@@ -1731,7 +1731,7 @@
         <v>1</v>
       </c>
       <c r="K36" t="n">
-        <v>-3.73316240801665</v>
+        <v>-3.73316240789031</v>
       </c>
       <c r="L36" t="n">
         <v>0.029</v>
@@ -1757,10 +1757,10 @@
         <v>0</v>
       </c>
       <c r="G37" t="n">
-        <v>1.4166008829141</v>
+        <v>1.41660088287921</v>
       </c>
       <c r="H37" t="n">
-        <v>0.132589089425266</v>
+        <v>0.132589089430697</v>
       </c>
       <c r="I37" t="e">
         <v>#NUM!</v>
@@ -1769,7 +1769,7 @@
         <v>1</v>
       </c>
       <c r="K37" t="n">
-        <v>3.72086263310626</v>
+        <v>3.72086263259902</v>
       </c>
       <c r="L37" t="n">
         <v>0.03</v>
@@ -1795,10 +1795,10 @@
         <v>0</v>
       </c>
       <c r="G38" t="n">
-        <v>0.915402483684154</v>
+        <v>0.915402483670631</v>
       </c>
       <c r="H38" t="n">
-        <v>0.0137974798971007</v>
+        <v>0.0137974798966685</v>
       </c>
       <c r="I38" t="e">
         <v>#NUM!</v>
@@ -1807,7 +1807,7 @@
         <v>1</v>
       </c>
       <c r="K38" t="n">
-        <v>-5.86438553033952</v>
+        <v>-5.86438553141674</v>
       </c>
       <c r="L38" t="n">
         <v>0</v>
@@ -1833,10 +1833,10 @@
         <v>0</v>
       </c>
       <c r="G39" t="n">
-        <v>0.726744661222566</v>
+        <v>0.726744661235944</v>
       </c>
       <c r="H39" t="n">
-        <v>0.0758158030668045</v>
+        <v>0.075815803072344</v>
       </c>
       <c r="I39" t="e">
         <v>#NUM!</v>
@@ -1845,7 +1845,7 @@
         <v>1</v>
       </c>
       <c r="K39" t="n">
-        <v>-3.05955241315849</v>
+        <v>-3.05955241281481</v>
       </c>
       <c r="L39" t="n">
         <v>0.339</v>
@@ -1871,10 +1871,10 @@
         <v>0</v>
       </c>
       <c r="G40" t="n">
-        <v>0.700830108862359</v>
+        <v>0.700830108869874</v>
       </c>
       <c r="H40" t="n">
-        <v>0.00916894982036112</v>
+        <v>0.00916894982053378</v>
       </c>
       <c r="I40" t="e">
         <v>#NUM!</v>
@@ -1883,7 +1883,7 @@
         <v>1</v>
       </c>
       <c r="K40" t="n">
-        <v>-27.171916500991</v>
+        <v>-27.1719164999511</v>
       </c>
       <c r="L40" t="n">
         <v>0</v>
@@ -1909,10 +1909,10 @@
         <v>0</v>
       </c>
       <c r="G41" t="n">
-        <v>1.13141782927354</v>
+        <v>1.13141782927834</v>
       </c>
       <c r="H41" t="n">
-        <v>0.0138229158065619</v>
+        <v>0.0138229158066658</v>
       </c>
       <c r="I41" t="e">
         <v>#NUM!</v>
@@ -1921,7 +1921,7 @@
         <v>1</v>
       </c>
       <c r="K41" t="n">
-        <v>10.1062560938062</v>
+        <v>10.1062560941205</v>
       </c>
       <c r="L41" t="n">
         <v>0</v>
@@ -1947,10 +1947,10 @@
         <v>0</v>
       </c>
       <c r="G42" t="n">
-        <v>0.900668737858972</v>
+        <v>0.900668737800778</v>
       </c>
       <c r="H42" t="n">
-        <v>0.0765048643211872</v>
+        <v>0.0765048643236415</v>
       </c>
       <c r="I42" t="e">
         <v>#NUM!</v>
@@ -1959,7 +1959,7 @@
         <v>1</v>
       </c>
       <c r="K42" t="n">
-        <v>-1.2316332725522</v>
+        <v>-1.23163327319377</v>
       </c>
       <c r="L42" t="n">
         <v>1</v>
@@ -1985,10 +1985,10 @@
         <v>0</v>
       </c>
       <c r="G43" t="n">
-        <v>0.868552331077003</v>
+        <v>0.86855233101421</v>
       </c>
       <c r="H43" t="n">
-        <v>0.0972531670238628</v>
+        <v>0.0972531670259449</v>
       </c>
       <c r="I43" t="e">
         <v>#NUM!</v>
@@ -1997,7 +1997,7 @@
         <v>1</v>
       </c>
       <c r="K43" t="n">
-        <v>-1.25860021593061</v>
+        <v>-1.25860021645834</v>
       </c>
       <c r="L43" t="n">
         <v>1</v>
@@ -2023,10 +2023,10 @@
         <v>0</v>
       </c>
       <c r="G44" t="n">
-        <v>1.08546164445406</v>
+        <v>1.0854616444827</v>
       </c>
       <c r="H44" t="n">
-        <v>0.0164432800365355</v>
+        <v>0.0164432800368264</v>
       </c>
       <c r="I44" t="e">
         <v>#NUM!</v>
@@ -2035,7 +2035,7 @@
         <v>1</v>
       </c>
       <c r="K44" t="n">
-        <v>5.41337794452499</v>
+        <v>5.41337794631377</v>
       </c>
       <c r="L44" t="n">
         <v>0</v>
@@ -2061,10 +2061,10 @@
         <v>0</v>
       </c>
       <c r="G45" t="n">
-        <v>0.69437546847765</v>
+        <v>0.694375468483133</v>
       </c>
       <c r="H45" t="n">
-        <v>0.0739814487897527</v>
+        <v>0.0739814487942718</v>
       </c>
       <c r="I45" t="e">
         <v>#NUM!</v>
@@ -2073,7 +2073,7 @@
         <v>1</v>
       </c>
       <c r="K45" t="n">
-        <v>-3.42340153523707</v>
+        <v>-3.42340153498087</v>
       </c>
       <c r="L45" t="n">
         <v>0.095</v>
@@ -2099,10 +2099,10 @@
         <v>0</v>
       </c>
       <c r="G46" t="n">
-        <v>0.669615149763734</v>
+        <v>0.669615149763876</v>
       </c>
       <c r="H46" t="n">
-        <v>0.0174290891727753</v>
+        <v>0.0174290891730255</v>
       </c>
       <c r="I46" t="e">
         <v>#NUM!</v>
@@ -2111,7 +2111,7 @@
         <v>1</v>
       </c>
       <c r="K46" t="n">
-        <v>-15.4081824217699</v>
+        <v>-15.4081824215438</v>
       </c>
       <c r="L46" t="n">
         <v>0</v>
@@ -2137,10 +2137,10 @@
         <v>0</v>
       </c>
       <c r="G47" t="n">
-        <v>1.0810245016787</v>
+        <v>1.08102450167193</v>
       </c>
       <c r="H47" t="n">
-        <v>0.0276618140437445</v>
+        <v>0.0276618140439398</v>
       </c>
       <c r="I47" t="e">
         <v>#NUM!</v>
@@ -2149,7 +2149,7 @@
         <v>1</v>
       </c>
       <c r="K47" t="n">
-        <v>3.04469397641184</v>
+        <v>3.04469397612631</v>
       </c>
       <c r="L47" t="n">
         <v>0.356</v>
@@ -2175,10 +2175,10 @@
         <v>0</v>
       </c>
       <c r="G48" t="n">
-        <v>1.28602301541536</v>
+        <v>1.28602301559359</v>
       </c>
       <c r="H48" t="n">
-        <v>0.201990213412559</v>
+        <v>0.201990213439608</v>
       </c>
       <c r="I48" t="e">
         <v>#NUM!</v>
@@ -2187,7 +2187,7 @@
         <v>1</v>
       </c>
       <c r="K48" t="n">
-        <v>1.60158702827409</v>
+        <v>1.60158702916394</v>
       </c>
       <c r="L48" t="n">
         <v>1</v>
@@ -2213,10 +2213,10 @@
         <v>0</v>
       </c>
       <c r="G49" t="n">
-        <v>1.02903524372754</v>
+        <v>1.02903524376861</v>
       </c>
       <c r="H49" t="n">
-        <v>0.114720091781507</v>
+        <v>0.114720091774135</v>
       </c>
       <c r="I49" t="e">
         <v>#NUM!</v>
@@ -2225,7 +2225,7 @@
         <v>1</v>
       </c>
       <c r="K49" t="n">
-        <v>0.256735716498083</v>
+        <v>0.256735716882777</v>
       </c>
       <c r="L49" t="n">
         <v>1</v>
@@ -2251,10 +2251,10 @@
         <v>0</v>
       </c>
       <c r="G50" t="n">
-        <v>1.66808992934494</v>
+        <v>1.66808992945516</v>
       </c>
       <c r="H50" t="n">
-        <v>0.188813550681997</v>
+        <v>0.188813550675585</v>
       </c>
       <c r="I50" t="e">
         <v>#NUM!</v>
@@ -2263,7 +2263,7 @@
         <v>1</v>
       </c>
       <c r="K50" t="n">
-        <v>4.5204750706758</v>
+        <v>4.5204750717118</v>
       </c>
       <c r="L50" t="n">
         <v>0.001</v>
@@ -2289,10 +2289,10 @@
         <v>0</v>
       </c>
       <c r="G51" t="n">
-        <v>1.04205828707977</v>
+        <v>1.04205828709326</v>
       </c>
       <c r="H51" t="n">
-        <v>0.145154393883516</v>
+        <v>0.145154393882823</v>
       </c>
       <c r="I51" t="e">
         <v>#NUM!</v>
@@ -2301,7 +2301,7 @@
         <v>1</v>
       </c>
       <c r="K51" t="n">
-        <v>0.295758127302929</v>
+        <v>0.295758127401115</v>
       </c>
       <c r="L51" t="n">
         <v>1</v>
@@ -2383,10 +2383,10 @@
         <v>0</v>
       </c>
       <c r="G54" t="n">
-        <v>0.987502576858034</v>
+        <v>0.987502576884656</v>
       </c>
       <c r="H54" t="n">
-        <v>0.175265198353641</v>
+        <v>0.175265198349305</v>
       </c>
       <c r="I54" t="e">
         <v>#NUM!</v>
@@ -2395,7 +2395,7 @@
         <v>1</v>
       </c>
       <c r="K54" t="n">
-        <v>-0.0708583512201663</v>
+        <v>-0.070858351071935</v>
       </c>
       <c r="L54" t="n">
         <v>1</v>
@@ -2421,10 +2421,10 @@
         <v>0</v>
       </c>
       <c r="G55" t="n">
-        <v>0.901742026018586</v>
+        <v>0.901742026062999</v>
       </c>
       <c r="H55" t="n">
-        <v>0.115335475603683</v>
+        <v>0.115335475599925</v>
       </c>
       <c r="I55" t="e">
         <v>#NUM!</v>
@@ -2433,7 +2433,7 @@
         <v>1</v>
       </c>
       <c r="K55" t="n">
-        <v>-0.808634927912254</v>
+        <v>-0.808634927593359</v>
       </c>
       <c r="L55" t="n">
         <v>1</v>
@@ -2487,10 +2487,10 @@
         <v>0</v>
       </c>
       <c r="G57" t="n">
-        <v>0.913154099189985</v>
+        <v>0.913154099210342</v>
       </c>
       <c r="H57" t="n">
-        <v>0.135922891322433</v>
+        <v>0.135922891323543</v>
       </c>
       <c r="I57" t="e">
         <v>#NUM!</v>
@@ -2499,7 +2499,7 @@
         <v>1</v>
       </c>
       <c r="K57" t="n">
-        <v>-0.610350646178583</v>
+        <v>-0.610350646037432</v>
       </c>
       <c r="L57" t="n">
         <v>1</v>
@@ -2581,10 +2581,10 @@
         <v>0</v>
       </c>
       <c r="G60" t="n">
-        <v>0.663928082244199</v>
+        <v>0.663928082139349</v>
       </c>
       <c r="H60" t="n">
-        <v>0.135440842488095</v>
+        <v>0.135440842417271</v>
       </c>
       <c r="I60" t="e">
         <v>#NUM!</v>
@@ -2593,7 +2593,7 @@
         <v>1</v>
       </c>
       <c r="K60" t="n">
-        <v>-2.00775939124946</v>
+        <v>-2.00775939275641</v>
       </c>
       <c r="L60" t="n">
         <v>1</v>
@@ -2619,10 +2619,10 @@
         <v>0</v>
       </c>
       <c r="G61" t="n">
-        <v>1.09648181604867</v>
+        <v>1.09648181604828</v>
       </c>
       <c r="H61" t="n">
-        <v>0.192456845531119</v>
+        <v>0.192456845517672</v>
       </c>
       <c r="I61" t="e">
         <v>#NUM!</v>
@@ -2631,7 +2631,7 @@
         <v>1</v>
       </c>
       <c r="K61" t="n">
-        <v>0.524758301050112</v>
+        <v>0.524758301084549</v>
       </c>
       <c r="L61" t="n">
         <v>1</v>
@@ -2657,10 +2657,10 @@
         <v>0</v>
       </c>
       <c r="G62" t="n">
-        <v>0.763898912207321</v>
+        <v>0.763898912274184</v>
       </c>
       <c r="H62" t="n">
-        <v>0.0928584310525138</v>
+        <v>0.092858431053611</v>
       </c>
       <c r="I62" t="e">
         <v>#NUM!</v>
@@ -2669,7 +2669,7 @@
         <v>1</v>
       </c>
       <c r="K62" t="n">
-        <v>-2.21555662122212</v>
+        <v>-2.21555662066981</v>
       </c>
       <c r="L62" t="n">
         <v>1</v>
@@ -2723,10 +2723,10 @@
         <v>0</v>
       </c>
       <c r="G64" t="n">
-        <v>1.11035843525329</v>
+        <v>1.11035843522296</v>
       </c>
       <c r="H64" t="n">
-        <v>0.164022119688661</v>
+        <v>0.164022119667154</v>
       </c>
       <c r="I64" t="e">
         <v>#NUM!</v>
@@ -2735,7 +2735,7 @@
         <v>1</v>
       </c>
       <c r="K64" t="n">
-        <v>0.708657568004375</v>
+        <v>0.708657567893016</v>
       </c>
       <c r="L64" t="n">
         <v>1</v>
@@ -2761,10 +2761,10 @@
         <v>0</v>
       </c>
       <c r="G65" t="n">
-        <v>0.773566500087362</v>
+        <v>0.773566500134218</v>
       </c>
       <c r="H65" t="n">
-        <v>0.104283192345617</v>
+        <v>0.104283192349616</v>
       </c>
       <c r="I65" t="e">
         <v>#NUM!</v>
@@ -2773,7 +2773,7 @@
         <v>1</v>
       </c>
       <c r="K65" t="n">
-        <v>-1.90450900395196</v>
+        <v>-1.90450900354498</v>
       </c>
       <c r="L65" t="n">
         <v>1</v>
@@ -2799,10 +2799,10 @@
         <v>0</v>
       </c>
       <c r="G66" t="n">
-        <v>0.847136864165157</v>
+        <v>0.847136864197583</v>
       </c>
       <c r="H66" t="n">
-        <v>0.0676169499719751</v>
+        <v>0.0676169499760599</v>
       </c>
       <c r="I66" t="e">
         <v>#NUM!</v>
@@ -2811,7 +2811,7 @@
         <v>1</v>
       </c>
       <c r="K66" t="n">
-        <v>-2.07838544456068</v>
+        <v>-2.07838544403512</v>
       </c>
       <c r="L66" t="n">
         <v>1</v>
@@ -2921,10 +2921,10 @@
         <v>0</v>
       </c>
       <c r="G70" t="n">
-        <v>1.95811797818843</v>
+        <v>1.95811797827485</v>
       </c>
       <c r="H70" t="n">
-        <v>0.281026041998921</v>
+        <v>0.281026042001463</v>
       </c>
       <c r="I70" t="e">
         <v>#NUM!</v>
@@ -2933,7 +2933,7 @@
         <v>1</v>
       </c>
       <c r="K70" t="n">
-        <v>4.68221216820307</v>
+        <v>4.68221216867486</v>
       </c>
       <c r="L70" t="n">
         <v>0</v>
@@ -2959,10 +2959,10 @@
         <v>0</v>
       </c>
       <c r="G71" t="n">
-        <v>1.23546566781543</v>
+        <v>1.2354656678617</v>
       </c>
       <c r="H71" t="n">
-        <v>0.177719857128329</v>
+        <v>0.17771985712861</v>
       </c>
       <c r="I71" t="e">
         <v>#NUM!</v>
@@ -2971,7 +2971,7 @@
         <v>1</v>
       </c>
       <c r="K71" t="n">
-        <v>1.46993530618326</v>
+        <v>1.46993530649633</v>
       </c>
       <c r="L71" t="n">
         <v>1</v>
@@ -2997,10 +2997,10 @@
         <v>0</v>
       </c>
       <c r="G72" t="n">
-        <v>1.17992792624951</v>
+        <v>1.17992792631445</v>
       </c>
       <c r="H72" t="n">
-        <v>0.168064734399258</v>
+        <v>0.168064734402442</v>
       </c>
       <c r="I72" t="e">
         <v>#NUM!</v>
@@ -3009,7 +3009,7 @@
         <v>1</v>
       </c>
       <c r="K72" t="n">
-        <v>1.16159429463698</v>
+        <v>1.16159429506532</v>
       </c>
       <c r="L72" t="n">
         <v>1</v>
@@ -3035,10 +3035,10 @@
         <v>0</v>
       </c>
       <c r="G73" t="n">
-        <v>2.36301766669016</v>
+        <v>2.3630176667881</v>
       </c>
       <c r="H73" t="n">
-        <v>0.337896249911925</v>
+        <v>0.337896249913983</v>
       </c>
       <c r="I73" t="e">
         <v>#NUM!</v>
@@ -3047,7 +3047,7 @@
         <v>1</v>
       </c>
       <c r="K73" t="n">
-        <v>6.01383463473155</v>
+        <v>6.01383463523403</v>
       </c>
       <c r="L73" t="n">
         <v>0</v>
@@ -3073,10 +3073,10 @@
         <v>0</v>
       </c>
       <c r="G74" t="n">
-        <v>1.25110120901795</v>
+        <v>1.25110120903108</v>
       </c>
       <c r="H74" t="n">
-        <v>0.13970846148669</v>
+        <v>0.139708461478049</v>
       </c>
       <c r="I74" t="e">
         <v>#NUM!</v>
@@ -3085,7 +3085,7 @@
         <v>1</v>
       </c>
       <c r="K74" t="n">
-        <v>2.00615523062334</v>
+        <v>2.00615523086242</v>
       </c>
       <c r="L74" t="n">
         <v>1</v>
@@ -3111,10 +3111,10 @@
         <v>0</v>
       </c>
       <c r="G75" t="n">
-        <v>1.19486060482365</v>
+        <v>1.1948606048572</v>
       </c>
       <c r="H75" t="n">
-        <v>0.130848203992801</v>
+        <v>0.13084820398677</v>
       </c>
       <c r="I75" t="e">
         <v>#NUM!</v>
@@ -3123,7 +3123,7 @@
         <v>1</v>
       </c>
       <c r="K75" t="n">
-        <v>1.62570417688063</v>
+        <v>1.62570417725762</v>
       </c>
       <c r="L75" t="n">
         <v>1</v>
@@ -3149,10 +3149,10 @@
         <v>0</v>
       </c>
       <c r="G76" t="n">
-        <v>1.30849832014504</v>
+        <v>1.30849832015261</v>
       </c>
       <c r="H76" t="n">
-        <v>0.13665196677563</v>
+        <v>0.136651966783791</v>
       </c>
       <c r="I76" t="e">
         <v>#NUM!</v>
@@ -3161,7 +3161,7 @@
         <v>1</v>
       </c>
       <c r="K76" t="n">
-        <v>2.57463719634452</v>
+        <v>2.57463719626107</v>
       </c>
       <c r="L76" t="n">
         <v>1</v>
@@ -3271,10 +3271,10 @@
         <v>0</v>
       </c>
       <c r="G80" t="n">
-        <v>1.45896228771617</v>
+        <v>1.45896228777569</v>
       </c>
       <c r="H80" t="n">
-        <v>0.162887545048089</v>
+        <v>0.162887545037813</v>
       </c>
       <c r="I80" t="e">
         <v>#NUM!</v>
@@ -3283,7 +3283,7 @@
         <v>1</v>
       </c>
       <c r="K80" t="n">
-        <v>3.38323684869576</v>
+        <v>3.38323684941258</v>
       </c>
       <c r="L80" t="n">
         <v>0.11</v>
@@ -3309,10 +3309,10 @@
         <v>0</v>
       </c>
       <c r="G81" t="n">
-        <v>1.15828072615174</v>
+        <v>1.15828072623742</v>
       </c>
       <c r="H81" t="n">
-        <v>0.175803958852529</v>
+        <v>0.175803958860239</v>
       </c>
       <c r="I81" t="e">
         <v>#NUM!</v>
@@ -3321,7 +3321,7 @@
         <v>1</v>
       </c>
       <c r="K81" t="n">
-        <v>0.968089872903285</v>
+        <v>0.968089873419828</v>
       </c>
       <c r="L81" t="n">
         <v>1</v>
@@ -3347,10 +3347,10 @@
         <v>0</v>
       </c>
       <c r="G82" t="n">
-        <v>1.11697828785769</v>
+        <v>1.11697828793173</v>
       </c>
       <c r="H82" t="n">
-        <v>0.124478880894225</v>
+        <v>0.124478880889549</v>
       </c>
       <c r="I82" t="e">
         <v>#NUM!</v>
@@ -3359,7 +3359,7 @@
         <v>1</v>
       </c>
       <c r="K82" t="n">
-        <v>0.992682837002429</v>
+        <v>0.992682837700365</v>
       </c>
       <c r="L82" t="n">
         <v>1</v>
@@ -3385,10 +3385,10 @@
         <v>0</v>
       </c>
       <c r="G83" t="n">
-        <v>1.80324608462537</v>
+        <v>1.80324608473322</v>
       </c>
       <c r="H83" t="n">
-        <v>0.200565687562567</v>
+        <v>0.200565687553644</v>
       </c>
       <c r="I83" t="e">
         <v>#NUM!</v>
@@ -3397,7 +3397,7 @@
         <v>1</v>
       </c>
       <c r="K83" t="n">
-        <v>5.30087187310232</v>
+        <v>5.30087187419295</v>
       </c>
       <c r="L83" t="n">
         <v>0</v>
@@ -3423,10 +3423,10 @@
         <v>0</v>
       </c>
       <c r="G84" t="n">
-        <v>1.17293944673752</v>
+        <v>1.17293944679267</v>
       </c>
       <c r="H84" t="n">
-        <v>0.13903504743427</v>
+        <v>0.13903504743272</v>
       </c>
       <c r="I84" t="e">
         <v>#NUM!</v>
@@ -3435,7 +3435,7 @@
         <v>1</v>
       </c>
       <c r="K84" t="n">
-        <v>1.34569685717675</v>
+        <v>1.34569685765167</v>
       </c>
       <c r="L84" t="n">
         <v>1</v>
@@ -3461,10 +3461,10 @@
         <v>0</v>
       </c>
       <c r="G85" t="n">
-        <v>1.13111430191059</v>
+        <v>1.13111430195508</v>
       </c>
       <c r="H85" t="n">
-        <v>0.157436893268949</v>
+        <v>0.157436893272382</v>
       </c>
       <c r="I85" t="e">
         <v>#NUM!</v>
@@ -3473,7 +3473,7 @@
         <v>1</v>
       </c>
       <c r="K85" t="n">
-        <v>0.885160781361655</v>
+        <v>0.885160781659748</v>
       </c>
       <c r="L85" t="n">
         <v>1</v>
@@ -3499,10 +3499,10 @@
         <v>0</v>
       </c>
       <c r="G86" t="n">
-        <v>1.23868939855163</v>
+        <v>1.23868939857273</v>
       </c>
       <c r="H86" t="n">
-        <v>0.0810905767719536</v>
+        <v>0.0810905767724046</v>
       </c>
       <c r="I86" t="e">
         <v>#NUM!</v>
@@ -3511,7 +3511,7 @@
         <v>1</v>
       </c>
       <c r="K86" t="n">
-        <v>3.26975448198011</v>
+        <v>3.2697544822779</v>
       </c>
       <c r="L86" t="n">
         <v>0.165</v>
@@ -3621,10 +3621,10 @@
         <v>0</v>
       </c>
       <c r="G90" t="n">
-        <v>1.93699144501971</v>
+        <v>1.93699144559405</v>
       </c>
       <c r="H90" t="n">
-        <v>0.396074603204476</v>
+        <v>0.396074603201308</v>
       </c>
       <c r="I90" t="e">
         <v>#NUM!</v>
@@ -3633,7 +3633,7 @@
         <v>1</v>
       </c>
       <c r="K90" t="n">
-        <v>3.23326641815879</v>
+        <v>3.23326642059343</v>
       </c>
       <c r="L90" t="n">
         <v>0.187</v>
@@ -3659,10 +3659,10 @@
         <v>0</v>
       </c>
       <c r="G91" t="n">
-        <v>1.54991974469466</v>
+        <v>1.54991974500128</v>
       </c>
       <c r="H91" t="n">
-        <v>0.266511135727783</v>
+        <v>0.266511135655166</v>
       </c>
       <c r="I91" t="e">
         <v>#NUM!</v>
@@ -3671,7 +3671,7 @@
         <v>1</v>
       </c>
       <c r="K91" t="n">
-        <v>2.54841027778335</v>
+        <v>2.54841028013238</v>
       </c>
       <c r="L91" t="n">
         <v>1</v>
@@ -3697,10 +3697,10 @@
         <v>0</v>
       </c>
       <c r="G92" t="n">
-        <v>2.51245575229547</v>
+        <v>2.51245575285826</v>
       </c>
       <c r="H92" t="n">
-        <v>0.434805364542669</v>
+        <v>0.434805364438372</v>
       </c>
       <c r="I92" t="e">
         <v>#NUM!</v>
@@ -3709,7 +3709,7 @@
         <v>1</v>
       </c>
       <c r="K92" t="n">
-        <v>5.32336267872661</v>
+        <v>5.32336268249034</v>
       </c>
       <c r="L92" t="n">
         <v>0</v>
@@ -3735,10 +3735,10 @@
         <v>0</v>
       </c>
       <c r="G93" t="n">
-        <v>0.93848819804036</v>
+        <v>0.938488198078147</v>
       </c>
       <c r="H93" t="n">
-        <v>0.128366299463585</v>
+        <v>0.128366299462874</v>
       </c>
       <c r="I93" t="e">
         <v>#NUM!</v>
@@ -3747,7 +3747,7 @@
         <v>1</v>
       </c>
       <c r="K93" t="n">
-        <v>-0.464139902600885</v>
+        <v>-0.464139902327777</v>
       </c>
       <c r="L93" t="n">
         <v>1</v>
@@ -3829,10 +3829,10 @@
         <v>0</v>
       </c>
       <c r="G96" t="n">
-        <v>1.48736377217257</v>
+        <v>1.48736377244756</v>
       </c>
       <c r="H96" t="n">
-        <v>0.328022298744835</v>
+        <v>0.328022298709448</v>
       </c>
       <c r="I96" t="e">
         <v>#NUM!</v>
@@ -3841,7 +3841,7 @@
         <v>1</v>
       </c>
       <c r="K96" t="n">
-        <v>1.80015584901985</v>
+        <v>1.80015585038519</v>
       </c>
       <c r="L96" t="n">
         <v>1</v>
@@ -3867,10 +3867,10 @@
         <v>0</v>
       </c>
       <c r="G97" t="n">
-        <v>1.35819232554606</v>
+        <v>1.35819232582745</v>
       </c>
       <c r="H97" t="n">
-        <v>0.248572723103392</v>
+        <v>0.248572723051361</v>
       </c>
       <c r="I97" t="e">
         <v>#NUM!</v>
@@ -3879,7 +3879,7 @@
         <v>1</v>
       </c>
       <c r="K97" t="n">
-        <v>1.67281784446532</v>
+        <v>1.67281784629405</v>
       </c>
       <c r="L97" t="n">
         <v>1</v>
@@ -3933,10 +3933,10 @@
         <v>0</v>
       </c>
       <c r="G99" t="n">
-        <v>0.822395786979979</v>
+        <v>0.822395787020778</v>
       </c>
       <c r="H99" t="n">
-        <v>0.120483569744594</v>
+        <v>0.120483569745935</v>
       </c>
       <c r="I99" t="e">
         <v>#NUM!</v>
@@ -3945,7 +3945,7 @@
         <v>1</v>
       </c>
       <c r="K99" t="n">
-        <v>-1.33467104948835</v>
+        <v>-1.33467104920108</v>
       </c>
       <c r="L99" t="n">
         <v>1</v>
@@ -4027,10 +4027,10 @@
         <v>0</v>
       </c>
       <c r="G102" t="n">
-        <v>1.65150691072196</v>
+        <v>1.65150691098218</v>
       </c>
       <c r="H102" t="n">
-        <v>0.361630369345433</v>
+        <v>0.361630369291159</v>
       </c>
       <c r="I102" t="e">
         <v>#NUM!</v>
@@ -4039,7 +4039,7 @@
         <v>1</v>
       </c>
       <c r="K102" t="n">
-        <v>2.29112795154251</v>
+        <v>2.29112795296695</v>
       </c>
       <c r="L102" t="n">
         <v>1</v>
@@ -4065,10 +4065,10 @@
         <v>0</v>
       </c>
       <c r="G103" t="n">
-        <v>1.15057478759627</v>
+        <v>1.15057478787869</v>
       </c>
       <c r="H103" t="n">
-        <v>0.205530046186997</v>
+        <v>0.205530046149029</v>
       </c>
       <c r="I103" t="e">
         <v>#NUM!</v>
@@ -4077,7 +4077,7 @@
         <v>1</v>
       </c>
       <c r="K103" t="n">
-        <v>0.785196623911994</v>
+        <v>0.785196625623844</v>
       </c>
       <c r="L103" t="n">
         <v>1</v>
@@ -4131,10 +4131,10 @@
         <v>0</v>
       </c>
       <c r="G105" t="n">
-        <v>0.696681788084856</v>
+        <v>0.696681788146086</v>
       </c>
       <c r="H105" t="n">
-        <v>0.0921145610371027</v>
+        <v>0.0921145610403699</v>
       </c>
       <c r="I105" t="e">
         <v>#NUM!</v>
@@ -4143,7 +4143,7 @@
         <v>1</v>
       </c>
       <c r="K105" t="n">
-        <v>-2.73354472590943</v>
+        <v>-2.73354472538801</v>
       </c>
       <c r="L105" t="n">
         <v>0.959</v>
@@ -4225,10 +4225,10 @@
         <v>0</v>
       </c>
       <c r="G108" t="n">
-        <v>2.94929229619212</v>
+        <v>2.94929229678805</v>
       </c>
       <c r="H108" t="n">
-        <v>0.572937647387888</v>
+        <v>0.572937647301204</v>
       </c>
       <c r="I108" t="e">
         <v>#NUM!</v>
@@ -4237,7 +4237,7 @@
         <v>1</v>
       </c>
       <c r="K108" t="n">
-        <v>5.5675378473208</v>
+        <v>5.56753785032824</v>
       </c>
       <c r="L108" t="n">
         <v>0</v>
@@ -4263,10 +4263,10 @@
         <v>0</v>
       </c>
       <c r="G109" t="n">
-        <v>1.86084261361461</v>
+        <v>1.86084261397817</v>
       </c>
       <c r="H109" t="n">
-        <v>0.361942104885768</v>
+        <v>0.361942104828727</v>
       </c>
       <c r="I109" t="e">
         <v>#NUM!</v>
@@ -4275,7 +4275,7 @@
         <v>1</v>
       </c>
       <c r="K109" t="n">
-        <v>3.1928807458759</v>
+        <v>3.19288074800736</v>
       </c>
       <c r="L109" t="n">
         <v>0.216</v>
@@ -4301,10 +4301,10 @@
         <v>0</v>
       </c>
       <c r="G110" t="n">
-        <v>1.77719237641091</v>
+        <v>1.77719237678938</v>
       </c>
       <c r="H110" t="n">
-        <v>0.34382450193311</v>
+        <v>0.343824501883746</v>
       </c>
       <c r="I110" t="e">
         <v>#NUM!</v>
@@ -4313,7 +4313,7 @@
         <v>1</v>
       </c>
       <c r="K110" t="n">
-        <v>2.97229389198161</v>
+        <v>2.97229389414213</v>
       </c>
       <c r="L110" t="n">
         <v>0.452</v>
@@ -4339,10 +4339,10 @@
         <v>0</v>
       </c>
       <c r="G111" t="n">
-        <v>3.55914703698437</v>
+        <v>3.55914703769396</v>
       </c>
       <c r="H111" t="n">
-        <v>0.690027849236143</v>
+        <v>0.69002784912891</v>
       </c>
       <c r="I111" t="e">
         <v>#NUM!</v>
@@ -4351,7 +4351,7 @@
         <v>1</v>
       </c>
       <c r="K111" t="n">
-        <v>6.5481583462319</v>
+        <v>6.54815834958336</v>
       </c>
       <c r="L111" t="n">
         <v>0</v>
@@ -4377,10 +4377,10 @@
         <v>0</v>
       </c>
       <c r="G112" t="n">
-        <v>1.12675436084075</v>
+        <v>1.12675436088335</v>
       </c>
       <c r="H112" t="n">
-        <v>0.122266316137736</v>
+        <v>0.122266316127672</v>
       </c>
       <c r="I112" t="e">
         <v>#NUM!</v>
@@ -4389,7 +4389,7 @@
         <v>1</v>
       </c>
       <c r="K112" t="n">
-        <v>1.09979822194658</v>
+        <v>1.09979822242711</v>
       </c>
       <c r="L112" t="n">
         <v>1</v>
@@ -4415,10 +4415,10 @@
         <v>0</v>
       </c>
       <c r="G113" t="n">
-        <v>1.07610350575766</v>
+        <v>1.07610350581727</v>
       </c>
       <c r="H113" t="n">
-        <v>0.114374830940692</v>
+        <v>0.114374830932836</v>
       </c>
       <c r="I113" t="e">
         <v>#NUM!</v>
@@ -4427,7 +4427,7 @@
         <v>1</v>
       </c>
       <c r="K113" t="n">
-        <v>0.690087047675175</v>
+        <v>0.690087048282006</v>
       </c>
       <c r="L113" t="n">
         <v>1</v>
@@ -4453,10 +4453,10 @@
         <v>0</v>
       </c>
       <c r="G114" t="n">
-        <v>1.54461265410112</v>
+        <v>1.54461265405093</v>
       </c>
       <c r="H114" t="n">
-        <v>0.129616232440292</v>
+        <v>0.129616232445161</v>
       </c>
       <c r="I114" t="e">
         <v>#NUM!</v>
@@ -4465,7 +4465,7 @@
         <v>1</v>
       </c>
       <c r="K114" t="n">
-        <v>5.18111139924434</v>
+        <v>5.18111139849417</v>
       </c>
       <c r="L114" t="n">
         <v>0</v>
@@ -4575,10 +4575,10 @@
         <v>0</v>
       </c>
       <c r="G118" t="n">
-        <v>2.19747036875532</v>
+        <v>2.19747036919199</v>
       </c>
       <c r="H118" t="n">
-        <v>0.378087164045551</v>
+        <v>0.378087163943076</v>
       </c>
       <c r="I118" t="e">
         <v>#NUM!</v>
@@ -4587,7 +4587,7 @@
         <v>1</v>
       </c>
       <c r="K118" t="n">
-        <v>4.57588533700682</v>
+        <v>4.57588534031132</v>
       </c>
       <c r="L118" t="n">
         <v>0.001</v>
@@ -4613,10 +4613,10 @@
         <v>0</v>
       </c>
       <c r="G119" t="n">
-        <v>1.74458764002953</v>
+        <v>1.7445876404341</v>
       </c>
       <c r="H119" t="n">
-        <v>0.349686432531529</v>
+        <v>0.349686432496781</v>
       </c>
       <c r="I119" t="e">
         <v>#NUM!</v>
@@ -4625,7 +4625,7 @@
         <v>1</v>
       </c>
       <c r="K119" t="n">
-        <v>2.77647261877365</v>
+        <v>2.77647262085036</v>
       </c>
       <c r="L119" t="n">
         <v>0.841</v>
@@ -4651,10 +4651,10 @@
         <v>0</v>
       </c>
       <c r="G120" t="n">
-        <v>1.68237843484809</v>
+        <v>1.6823784352253</v>
       </c>
       <c r="H120" t="n">
-        <v>0.289245372318634</v>
+        <v>0.289245372247456</v>
       </c>
       <c r="I120" t="e">
         <v>#NUM!</v>
@@ -4663,7 +4663,7 @@
         <v>1</v>
       </c>
       <c r="K120" t="n">
-        <v>3.02576183269578</v>
+        <v>3.02576183542291</v>
       </c>
       <c r="L120" t="n">
         <v>0.379</v>
@@ -4689,10 +4689,10 @@
         <v>0</v>
       </c>
       <c r="G121" t="n">
-        <v>2.716026227615</v>
+        <v>2.71602622820637</v>
       </c>
       <c r="H121" t="n">
-        <v>0.466560861399594</v>
+        <v>0.466560861281385</v>
       </c>
       <c r="I121" t="e">
         <v>#NUM!</v>
@@ -4701,7 +4701,7 @@
         <v>1</v>
       </c>
       <c r="K121" t="n">
-        <v>5.81654353673321</v>
+        <v>5.81654354074088</v>
       </c>
       <c r="L121" t="n">
         <v>0</v>
@@ -4727,10 +4727,10 @@
         <v>0</v>
       </c>
       <c r="G122" t="n">
-        <v>1.05636108980427</v>
+        <v>1.05636108988279</v>
       </c>
       <c r="H122" t="n">
-        <v>0.122081055126298</v>
+        <v>0.122081055123229</v>
       </c>
       <c r="I122" t="e">
         <v>#NUM!</v>
@@ -4739,7 +4739,7 @@
         <v>1</v>
       </c>
       <c r="K122" t="n">
-        <v>0.474441757250303</v>
+        <v>0.4744417579407</v>
       </c>
       <c r="L122" t="n">
         <v>1</v>
@@ -4765,10 +4765,10 @@
         <v>0</v>
       </c>
       <c r="G123" t="n">
-        <v>1.01869294274562</v>
+        <v>1.01869294281351</v>
       </c>
       <c r="H123" t="n">
-        <v>0.139223347567045</v>
+        <v>0.139223347569969</v>
       </c>
       <c r="I123" t="e">
         <v>#NUM!</v>
@@ -4777,7 +4777,7 @@
         <v>1</v>
       </c>
       <c r="K123" t="n">
-        <v>0.135513026787711</v>
+        <v>0.135513027281559</v>
       </c>
       <c r="L123" t="n">
         <v>1</v>
@@ -4803,10 +4803,10 @@
         <v>0</v>
       </c>
       <c r="G124" t="n">
-        <v>1.4622069360331</v>
+        <v>1.46220693600205</v>
       </c>
       <c r="H124" t="n">
-        <v>0.0756678640047479</v>
+        <v>0.075667864007999</v>
       </c>
       <c r="I124" t="e">
         <v>#NUM!</v>
@@ -4815,7 +4815,7 @@
         <v>1</v>
       </c>
       <c r="K124" t="n">
-        <v>7.34209947195673</v>
+        <v>7.34209947107491</v>
       </c>
       <c r="L124" t="n">
         <v>0</v>
@@ -4925,10 +4925,10 @@
         <v>0</v>
       </c>
       <c r="G128" t="n">
-        <v>0.656764827114827</v>
+        <v>0.656764827176862</v>
       </c>
       <c r="H128" t="n">
-        <v>0.0495691252876188</v>
+        <v>0.0495691252977727</v>
       </c>
       <c r="I128" t="e">
         <v>#NUM!</v>
@@ -4937,7 +4937,7 @@
         <v>1</v>
       </c>
       <c r="K128" t="n">
-        <v>-5.57046665569595</v>
+        <v>-5.57046665382957</v>
       </c>
       <c r="L128" t="n">
         <v>0</v>
@@ -4963,10 +4963,10 @@
         <v>0</v>
       </c>
       <c r="G129" t="n">
-        <v>0.525522596283787</v>
+        <v>0.525522596281565</v>
       </c>
       <c r="H129" t="n">
-        <v>0.0484371686370213</v>
+        <v>0.0484371686400236</v>
       </c>
       <c r="I129" t="e">
         <v>#NUM!</v>
@@ -4975,7 +4975,7 @@
         <v>1</v>
       </c>
       <c r="K129" t="n">
-        <v>-6.98020395084547</v>
+        <v>-6.98020395042918</v>
       </c>
       <c r="L129" t="n">
         <v>0</v>
@@ -5001,10 +5001,10 @@
         <v>0</v>
       </c>
       <c r="G130" t="n">
-        <v>0.851884282727534</v>
+        <v>0.851884282746228</v>
       </c>
       <c r="H130" t="n">
-        <v>0.0804141515753738</v>
+        <v>0.0804141515823267</v>
       </c>
       <c r="I130" t="e">
         <v>#NUM!</v>
@@ -5013,7 +5013,7 @@
         <v>1</v>
       </c>
       <c r="K130" t="n">
-        <v>-1.6982203913314</v>
+        <v>-1.69822039098935</v>
       </c>
       <c r="L130" t="n">
         <v>1</v>
@@ -5039,10 +5039,10 @@
         <v>0</v>
       </c>
       <c r="G131" t="n">
-        <v>0.832912860741082</v>
+        <v>0.832912860743127</v>
       </c>
       <c r="H131" t="n">
-        <v>0.0772032439780711</v>
+        <v>0.0772032439831388</v>
       </c>
       <c r="I131" t="e">
         <v>#NUM!</v>
@@ -5051,7 +5051,7 @@
         <v>1</v>
       </c>
       <c r="K131" t="n">
-        <v>-1.97243442235871</v>
+        <v>-1.97243442220759</v>
       </c>
       <c r="L131" t="n">
         <v>1</v>
@@ -5077,10 +5077,10 @@
         <v>0</v>
       </c>
       <c r="G132" t="n">
-        <v>0.544229115822342</v>
+        <v>0.544229115875209</v>
       </c>
       <c r="H132" t="n">
-        <v>0.0405191110878029</v>
+        <v>0.0405191110963359</v>
       </c>
       <c r="I132" t="e">
         <v>#NUM!</v>
@@ -5089,7 +5089,7 @@
         <v>1</v>
       </c>
       <c r="K132" t="n">
-        <v>-8.17147256241829</v>
+        <v>-8.17147256018649</v>
       </c>
       <c r="L132" t="n">
         <v>0</v>
@@ -5115,10 +5115,10 @@
         <v>0</v>
       </c>
       <c r="G133" t="n">
-        <v>0.435475053036271</v>
+        <v>0.4354750530356</v>
       </c>
       <c r="H133" t="n">
-        <v>0.0397813466419573</v>
+        <v>0.039781346644576</v>
       </c>
       <c r="I133" t="e">
         <v>#NUM!</v>
@@ -5127,7 +5127,7 @@
         <v>1</v>
       </c>
       <c r="K133" t="n">
-        <v>-9.10019844963145</v>
+        <v>-9.10019844903527</v>
       </c>
       <c r="L133" t="n">
         <v>0</v>
@@ -5153,10 +5153,10 @@
         <v>0</v>
       </c>
       <c r="G134" t="n">
-        <v>0.504312093478469</v>
+        <v>0.504312093469808</v>
       </c>
       <c r="H134" t="n">
-        <v>0.0564585561414966</v>
+        <v>0.0564585561365325</v>
       </c>
       <c r="I134" t="e">
         <v>#NUM!</v>
@@ -5165,7 +5165,7 @@
         <v>1</v>
       </c>
       <c r="K134" t="n">
-        <v>-6.11478392126892</v>
+        <v>-6.11478392185495</v>
       </c>
       <c r="L134" t="n">
         <v>0</v>
@@ -5191,10 +5191,10 @@
         <v>0</v>
       </c>
       <c r="G135" t="n">
-        <v>0.460514655430947</v>
+        <v>0.460514655433304</v>
       </c>
       <c r="H135" t="n">
-        <v>0.0487975229268272</v>
+        <v>0.0487975229296668</v>
       </c>
       <c r="I135" t="e">
         <v>#NUM!</v>
@@ -5203,7 +5203,7 @@
         <v>1</v>
       </c>
       <c r="K135" t="n">
-        <v>-7.31774736266344</v>
+        <v>-7.31774736222676</v>
       </c>
       <c r="L135" t="n">
         <v>0</v>
@@ -5257,10 +5257,10 @@
         <v>0</v>
       </c>
       <c r="G137" t="n">
-        <v>0.729880278755993</v>
+        <v>0.729880278764607</v>
       </c>
       <c r="H137" t="n">
-        <v>0.0776181782174944</v>
+        <v>0.0776181782223809</v>
       </c>
       <c r="I137" t="e">
         <v>#NUM!</v>
@@ -5269,7 +5269,7 @@
         <v>1</v>
       </c>
       <c r="K137" t="n">
-        <v>-2.96091563697038</v>
+        <v>-2.96091563670794</v>
       </c>
       <c r="L137" t="n">
         <v>0.469</v>
@@ -5295,10 +5295,10 @@
         <v>0</v>
       </c>
       <c r="G138" t="n">
-        <v>0.417898939469722</v>
+        <v>0.417898939463668</v>
       </c>
       <c r="H138" t="n">
-        <v>0.0464968868224725</v>
+        <v>0.0464968868184691</v>
       </c>
       <c r="I138" t="e">
         <v>#NUM!</v>
@@ -5307,7 +5307,7 @@
         <v>1</v>
       </c>
       <c r="K138" t="n">
-        <v>-7.84188767446679</v>
+        <v>-7.84188767515858</v>
       </c>
       <c r="L138" t="n">
         <v>0</v>
@@ -5333,10 +5333,10 @@
         <v>0</v>
       </c>
       <c r="G139" t="n">
-        <v>0.381606129623924</v>
+        <v>0.381606129626903</v>
       </c>
       <c r="H139" t="n">
-        <v>0.0401654606529056</v>
+        <v>0.0401654606553792</v>
       </c>
       <c r="I139" t="e">
         <v>#NUM!</v>
@@ -5345,7 +5345,7 @@
         <v>1</v>
       </c>
       <c r="K139" t="n">
-        <v>-9.15280119387308</v>
+        <v>-9.1528011933067</v>
       </c>
       <c r="L139" t="n">
         <v>0</v>
@@ -5371,10 +5371,10 @@
         <v>0</v>
       </c>
       <c r="G140" t="n">
-        <v>0.559967186994062</v>
+        <v>0.559967186969149</v>
       </c>
       <c r="H140" t="n">
-        <v>0.0609250618643726</v>
+        <v>0.0609250618544619</v>
       </c>
       <c r="I140" t="e">
         <v>#NUM!</v>
@@ -5383,7 +5383,7 @@
         <v>1</v>
       </c>
       <c r="K140" t="n">
-        <v>-5.32969739975576</v>
+        <v>-5.32969740079455</v>
       </c>
       <c r="L140" t="n">
         <v>0</v>
@@ -5409,10 +5409,10 @@
         <v>0</v>
       </c>
       <c r="G141" t="n">
-        <v>0.39011894110387</v>
+        <v>0.3901189411208</v>
       </c>
       <c r="H141" t="n">
-        <v>0.0334873532324707</v>
+        <v>0.033487353236214</v>
       </c>
       <c r="I141" t="e">
         <v>#NUM!</v>
@@ -5421,7 +5421,7 @@
         <v>1</v>
       </c>
       <c r="K141" t="n">
-        <v>-10.965941820349</v>
+        <v>-10.9659418190935</v>
       </c>
       <c r="L141" t="n">
         <v>0</v>
@@ -5475,10 +5475,10 @@
         <v>0</v>
       </c>
       <c r="G143" t="n">
-        <v>0.618308490561343</v>
+        <v>0.618308490592307</v>
       </c>
       <c r="H143" t="n">
-        <v>0.053377320761345</v>
+        <v>0.0533773207674808</v>
       </c>
       <c r="I143" t="e">
         <v>#NUM!</v>
@@ -5487,7 +5487,7 @@
         <v>1</v>
       </c>
       <c r="K143" t="n">
-        <v>-5.56908421385742</v>
+        <v>-5.56908421291603</v>
       </c>
       <c r="L143" t="n">
         <v>0</v>
@@ -5513,10 +5513,10 @@
         <v>0</v>
       </c>
       <c r="G144" t="n">
-        <v>0.464017612523608</v>
+        <v>0.46401761250421</v>
       </c>
       <c r="H144" t="n">
-        <v>0.0501573815850425</v>
+        <v>0.0501573815769409</v>
       </c>
       <c r="I144" t="e">
         <v>#NUM!</v>
@@ -5525,7 +5525,7 @@
         <v>1</v>
       </c>
       <c r="K144" t="n">
-        <v>-7.10339968393425</v>
+        <v>-7.10339968517139</v>
       </c>
       <c r="L144" t="n">
         <v>0</v>
@@ -5551,10 +5551,10 @@
         <v>0</v>
       </c>
       <c r="G145" t="n">
-        <v>0.323272619995813</v>
+        <v>0.323272620010711</v>
       </c>
       <c r="H145" t="n">
-        <v>0.0274627420954394</v>
+        <v>0.0274627420986216</v>
       </c>
       <c r="I145" t="e">
         <v>#NUM!</v>
@@ -5563,7 +5563,7 @@
         <v>1</v>
       </c>
       <c r="K145" t="n">
-        <v>-13.292868100798</v>
+        <v>-13.2928680993278</v>
       </c>
       <c r="L145" t="n">
         <v>0</v>
@@ -5589,10 +5589,10 @@
         <v>0</v>
       </c>
       <c r="G146" t="n">
-        <v>0.630945469873289</v>
+        <v>0.630945469869072</v>
       </c>
       <c r="H146" t="n">
-        <v>0.0182531305009342</v>
+        <v>0.0182531305006612</v>
       </c>
       <c r="I146" t="e">
         <v>#NUM!</v>
@@ -5601,7 +5601,7 @@
         <v>1</v>
       </c>
       <c r="K146" t="n">
-        <v>-15.9190776160157</v>
+        <v>-15.9190776163784</v>
       </c>
       <c r="L146" t="n">
         <v>0</v>
@@ -5627,10 +5627,10 @@
         <v>0</v>
       </c>
       <c r="G147" t="n">
-        <v>0.602582653033566</v>
+        <v>0.602582653040137</v>
       </c>
       <c r="H147" t="n">
-        <v>0.0153422796469165</v>
+        <v>0.0153422796471957</v>
       </c>
       <c r="I147" t="e">
         <v>#NUM!</v>
@@ -5639,7 +5639,7 @@
         <v>1</v>
       </c>
       <c r="K147" t="n">
-        <v>-19.8944656948968</v>
+        <v>-19.8944656943234</v>
       </c>
       <c r="L147" t="n">
         <v>0</v>
@@ -5665,10 +5665,10 @@
         <v>0</v>
       </c>
       <c r="G148" t="n">
-        <v>1.20678002705247</v>
+        <v>1.20678002704923</v>
       </c>
       <c r="H148" t="n">
-        <v>0.0252774723515188</v>
+        <v>0.0252774723513906</v>
       </c>
       <c r="I148" t="e">
         <v>#NUM!</v>
@@ -5677,7 +5677,7 @@
         <v>1</v>
       </c>
       <c r="K148" t="n">
-        <v>8.97325313305902</v>
+        <v>8.97325313295211</v>
       </c>
       <c r="L148" t="n">
         <v>0</v>
@@ -5703,10 +5703,10 @@
         <v>0</v>
       </c>
       <c r="G149" t="n">
-        <v>0.955047118659211</v>
+        <v>0.955047118676009</v>
       </c>
       <c r="H149" t="n">
-        <v>0.0258645772188469</v>
+        <v>0.0258645772190148</v>
       </c>
       <c r="I149" t="e">
         <v>#NUM!</v>
@@ -5715,7 +5715,7 @@
         <v>1</v>
       </c>
       <c r="K149" t="n">
-        <v>-1.6983463755943</v>
+        <v>-1.69834637496368</v>
       </c>
       <c r="L149" t="n">
         <v>1</v>
@@ -5741,10 +5741,10 @@
         <v>0</v>
       </c>
       <c r="G150" t="n">
-        <v>0.52283386841789</v>
+        <v>0.522833868415801</v>
       </c>
       <c r="H150" t="n">
-        <v>0.0141458938158284</v>
+        <v>0.0141458938156214</v>
       </c>
       <c r="I150" t="e">
         <v>#NUM!</v>
@@ -5753,7 +5753,7 @@
         <v>1</v>
       </c>
       <c r="K150" t="n">
-        <v>-23.9683213141566</v>
+        <v>-23.9683213145593</v>
       </c>
       <c r="L150" t="n">
         <v>0</v>
@@ -5779,10 +5779,10 @@
         <v>0</v>
       </c>
       <c r="G151" t="n">
-        <v>0.499330979569955</v>
+        <v>0.499330979576742</v>
       </c>
       <c r="H151" t="n">
-        <v>0.0109918838313895</v>
+        <v>0.0109918838316461</v>
       </c>
       <c r="I151" t="e">
         <v>#NUM!</v>
@@ -5791,7 +5791,7 @@
         <v>1</v>
       </c>
       <c r="K151" t="n">
-        <v>-31.5485897246112</v>
+        <v>-31.5485897236861</v>
       </c>
       <c r="L151" t="n">
         <v>0</v>
@@ -5817,10 +5817,10 @@
         <v>0</v>
       </c>
       <c r="G152" t="n">
-        <v>0.745083955087295</v>
+        <v>0.745083955084807</v>
       </c>
       <c r="H152" t="n">
-        <v>0.0688704097008529</v>
+        <v>0.0688704097051538</v>
       </c>
       <c r="I152" t="e">
         <v>#NUM!</v>
@@ -5829,7 +5829,7 @@
         <v>1</v>
       </c>
       <c r="K152" t="n">
-        <v>-3.18347451731029</v>
+        <v>-3.18347451713699</v>
       </c>
       <c r="L152" t="n">
         <v>0.223</v>
@@ -5855,10 +5855,10 @@
         <v>0</v>
       </c>
       <c r="G153" t="n">
-        <v>0.591527547907678</v>
+        <v>0.59152754792533</v>
       </c>
       <c r="H153" t="n">
-        <v>0.0377260183702753</v>
+        <v>0.0377260183718564</v>
       </c>
       <c r="I153" t="e">
         <v>#NUM!</v>
@@ -5867,7 +5867,7 @@
         <v>1</v>
       </c>
       <c r="K153" t="n">
-        <v>-8.23250880621333</v>
+        <v>-8.23250880564606</v>
       </c>
       <c r="L153" t="n">
         <v>0</v>
@@ -5893,10 +5893,10 @@
         <v>0</v>
       </c>
       <c r="G154" t="n">
-        <v>0.570434621559969</v>
+        <v>0.570434621572608</v>
       </c>
       <c r="H154" t="n">
-        <v>0.0524821796381841</v>
+        <v>0.0524821796428621</v>
       </c>
       <c r="I154" t="e">
         <v>#NUM!</v>
@@ -5905,7 +5905,7 @@
         <v>1</v>
       </c>
       <c r="K154" t="n">
-        <v>-6.10144828854646</v>
+        <v>-6.10144828789697</v>
       </c>
       <c r="L154" t="n">
         <v>0</v>
@@ -5931,10 +5931,10 @@
         <v>0</v>
       </c>
       <c r="G155" t="n">
-        <v>0.92090778222345</v>
+        <v>0.920907782237887</v>
       </c>
       <c r="H155" t="n">
-        <v>0.0846834436677906</v>
+        <v>0.0846834436747939</v>
       </c>
       <c r="I155" t="e">
         <v>#NUM!</v>
@@ -5943,7 +5943,7 @@
         <v>1</v>
       </c>
       <c r="K155" t="n">
-        <v>-0.896025708689697</v>
+        <v>-0.896025708459161</v>
       </c>
       <c r="L155" t="n">
         <v>1</v>
@@ -5969,10 +5969,10 @@
         <v>0</v>
       </c>
       <c r="G156" t="n">
-        <v>0.937525628049081</v>
+        <v>0.937525628083325</v>
       </c>
       <c r="H156" t="n">
-        <v>0.059328383943552</v>
+        <v>0.0593283839462175</v>
       </c>
       <c r="I156" t="e">
         <v>#NUM!</v>
@@ -5981,7 +5981,7 @@
         <v>1</v>
       </c>
       <c r="K156" t="n">
-        <v>-1.01942586572112</v>
+        <v>-1.01942586513537</v>
       </c>
       <c r="L156" t="n">
         <v>1</v>
@@ -6007,10 +6007,10 @@
         <v>0</v>
       </c>
       <c r="G157" t="n">
-        <v>0.904094963506954</v>
+        <v>0.904094963533028</v>
       </c>
       <c r="H157" t="n">
-        <v>0.0836523328519719</v>
+        <v>0.083652332859732</v>
       </c>
       <c r="I157" t="e">
         <v>#NUM!</v>
@@ -6019,7 +6019,7 @@
         <v>1</v>
       </c>
       <c r="K157" t="n">
-        <v>-1.08964858578596</v>
+        <v>-1.08964858540461</v>
       </c>
       <c r="L157" t="n">
         <v>1</v>
@@ -6045,10 +6045,10 @@
         <v>0</v>
       </c>
       <c r="G158" t="n">
-        <v>0.946649590206828</v>
+        <v>0.94664959021748</v>
       </c>
       <c r="H158" t="n">
-        <v>0.0854924515110234</v>
+        <v>0.0854924515178276</v>
       </c>
       <c r="I158" t="e">
         <v>#NUM!</v>
@@ -6057,7 +6057,7 @@
         <v>1</v>
       </c>
       <c r="K158" t="n">
-        <v>-0.607086005915674</v>
+        <v>-0.607086005749599</v>
       </c>
       <c r="L158" t="n">
         <v>1</v>
@@ -6083,10 +6083,10 @@
         <v>0</v>
       </c>
       <c r="G159" t="n">
-        <v>0.490170150853813</v>
+        <v>0.490170150869758</v>
       </c>
       <c r="H159" t="n">
-        <v>0.0306662795567281</v>
+        <v>0.0306662795581112</v>
       </c>
       <c r="I159" t="e">
         <v>#NUM!</v>
@@ -6095,7 +6095,7 @@
         <v>1</v>
       </c>
       <c r="K159" t="n">
-        <v>-11.3966430493594</v>
+        <v>-11.3966430486961</v>
       </c>
       <c r="L159" t="n">
         <v>0</v>
@@ -6121,10 +6121,10 @@
         <v>0</v>
       </c>
       <c r="G160" t="n">
-        <v>0.472691467187472</v>
+        <v>0.472691467199215</v>
       </c>
       <c r="H160" t="n">
-        <v>0.0431022175431642</v>
+        <v>0.0431022175471725</v>
       </c>
       <c r="I160" t="e">
         <v>#NUM!</v>
@@ -6133,7 +6133,7 @@
         <v>1</v>
       </c>
       <c r="K160" t="n">
-        <v>-8.21752555700523</v>
+        <v>-8.21752555617274</v>
       </c>
       <c r="L160" t="n">
         <v>0</v>
@@ -6159,10 +6159,10 @@
         <v>0</v>
       </c>
       <c r="G161" t="n">
-        <v>0.763111554367323</v>
+        <v>0.763111554381337</v>
       </c>
       <c r="H161" t="n">
-        <v>0.0695471095540686</v>
+        <v>0.0695471095600888</v>
       </c>
       <c r="I161" t="e">
         <v>#NUM!</v>
@@ -6171,7 +6171,7 @@
         <v>1</v>
       </c>
       <c r="K161" t="n">
-        <v>-2.96644984879555</v>
+        <v>-2.96644984839174</v>
       </c>
       <c r="L161" t="n">
         <v>0.461</v>
@@ -6197,10 +6197,10 @@
         <v>0</v>
       </c>
       <c r="G162" t="n">
-        <v>0.881464192901429</v>
+        <v>0.881464192987631</v>
       </c>
       <c r="H162" t="n">
-        <v>0.0990083386006116</v>
+        <v>0.0990083386194748</v>
       </c>
       <c r="I162" t="e">
         <v>#NUM!</v>
@@ -6209,7 +6209,7 @@
         <v>1</v>
       </c>
       <c r="K162" t="n">
-        <v>-1.12329053175302</v>
+        <v>-1.12329053077821</v>
       </c>
       <c r="L162" t="n">
         <v>1</v>
@@ -6235,10 +6235,10 @@
         <v>0</v>
       </c>
       <c r="G163" t="n">
-        <v>0.705319974609057</v>
+        <v>0.705319974608431</v>
       </c>
       <c r="H163" t="n">
-        <v>0.012006573465501</v>
+        <v>0.0120065734651968</v>
       </c>
       <c r="I163" t="e">
         <v>#NUM!</v>
@@ -6247,7 +6247,7 @@
         <v>1</v>
       </c>
       <c r="K163" t="n">
-        <v>-20.5079179095833</v>
+        <v>-20.5079179101367</v>
       </c>
       <c r="L163" t="n">
         <v>0</v>
@@ -6273,10 +6273,10 @@
         <v>0</v>
       </c>
       <c r="G164" t="n">
-        <v>1.14333999130034</v>
+        <v>1.14333999132925</v>
       </c>
       <c r="H164" t="n">
-        <v>0.0310379005586971</v>
+        <v>0.031037900559667</v>
       </c>
       <c r="I164" t="e">
         <v>#NUM!</v>
@@ -6285,7 +6285,7 @@
         <v>1</v>
       </c>
       <c r="K164" t="n">
-        <v>4.93444237379205</v>
+        <v>4.93444237469402</v>
       </c>
       <c r="L164" t="n">
         <v>0</v>
@@ -6311,10 +6311,10 @@
         <v>0</v>
       </c>
       <c r="G165" t="n">
-        <v>0.888416098527684</v>
+        <v>0.888416098497416</v>
       </c>
       <c r="H165" t="n">
-        <v>0.0929165792811648</v>
+        <v>0.0929165792830225</v>
       </c>
       <c r="I165" t="e">
         <v>#NUM!</v>
@@ -6323,7 +6323,7 @@
         <v>1</v>
       </c>
       <c r="K165" t="n">
-        <v>-1.1312621539305</v>
+        <v>-1.13126215419509</v>
       </c>
       <c r="L165" t="n">
         <v>1</v>
@@ -6349,10 +6349,10 @@
         <v>0</v>
       </c>
       <c r="G166" t="n">
-        <v>0.713171112018542</v>
+        <v>0.713171112074724</v>
       </c>
       <c r="H166" t="n">
-        <v>0.0798256901550254</v>
+        <v>0.0798256901687974</v>
       </c>
       <c r="I166" t="e">
         <v>#NUM!</v>
@@ -6361,7 +6361,7 @@
         <v>1</v>
       </c>
       <c r="K166" t="n">
-        <v>-3.02003040454852</v>
+        <v>-3.02003040356159</v>
       </c>
       <c r="L166" t="n">
         <v>0.387</v>
@@ -6387,10 +6387,10 @@
         <v>0</v>
       </c>
       <c r="G167" t="n">
-        <v>0.570657134653547</v>
+        <v>0.570657134642188</v>
       </c>
       <c r="H167" t="n">
-        <v>0.0083007445355511</v>
+        <v>0.00830074453527493</v>
       </c>
       <c r="I167" t="e">
         <v>#NUM!</v>
@@ -6399,7 +6399,7 @@
         <v>1</v>
       </c>
       <c r="K167" t="n">
-        <v>-38.5651740629118</v>
+        <v>-38.5651740647956</v>
       </c>
       <c r="L167" t="n">
         <v>0</v>
@@ -6425,10 +6425,10 @@
         <v>0</v>
       </c>
       <c r="G168" t="n">
-        <v>0.676852709060663</v>
+        <v>0.676852709051299</v>
       </c>
       <c r="H168" t="n">
-        <v>0.0943980772330658</v>
+        <v>0.0943980772300894</v>
       </c>
       <c r="I168" t="e">
         <v>#NUM!</v>
@@ -6437,7 +6437,7 @@
         <v>1</v>
       </c>
       <c r="K168" t="n">
-        <v>-2.79853889961062</v>
+        <v>-2.79853889975934</v>
       </c>
       <c r="L168" t="n">
         <v>0.785</v>
@@ -6463,10 +6463,10 @@
         <v>0</v>
       </c>
       <c r="G169" t="n">
-        <v>0.61807082582659</v>
+        <v>0.618070825831819</v>
       </c>
       <c r="H169" t="n">
-        <v>0.0407207744358378</v>
+        <v>0.0407207744356785</v>
       </c>
       <c r="I169" t="e">
         <v>#NUM!</v>
@@ -6475,7 +6475,7 @@
         <v>1</v>
       </c>
       <c r="K169" t="n">
-        <v>-7.30305737201055</v>
+        <v>-7.3030573719725</v>
       </c>
       <c r="L169" t="n">
         <v>0</v>
@@ -6529,10 +6529,10 @@
         <v>0</v>
       </c>
       <c r="G171" t="n">
-        <v>0.77851768199107</v>
+        <v>0.778517681971823</v>
       </c>
       <c r="H171" t="n">
-        <v>0.0910982787666929</v>
+        <v>0.0910982787685799</v>
       </c>
       <c r="I171" t="e">
         <v>#NUM!</v>
@@ -6541,7 +6541,7 @@
         <v>1</v>
       </c>
       <c r="K171" t="n">
-        <v>-2.13958455369013</v>
+        <v>-2.13958455380419</v>
       </c>
       <c r="L171" t="n">
         <v>1</v>
@@ -6567,10 +6567,10 @@
         <v>0</v>
       </c>
       <c r="G172" t="n">
-        <v>0.547624966596386</v>
+        <v>0.547624966578396</v>
       </c>
       <c r="H172" t="n">
-        <v>0.076201108577257</v>
+        <v>0.0762011085734174</v>
       </c>
       <c r="I172" t="e">
         <v>#NUM!</v>
@@ -6579,7 +6579,7 @@
         <v>1</v>
       </c>
       <c r="K172" t="n">
-        <v>-4.32750089528866</v>
+        <v>-4.32750089560064</v>
       </c>
       <c r="L172" t="n">
         <v>0.002</v>
@@ -6605,10 +6605,10 @@
         <v>0</v>
       </c>
       <c r="G173" t="n">
-        <v>0.500065983066269</v>
+        <v>0.500065983060989</v>
       </c>
       <c r="H173" t="n">
-        <v>0.0325900661023443</v>
+        <v>0.0325900661016223</v>
       </c>
       <c r="I173" t="e">
         <v>#NUM!</v>
@@ -6617,7 +6617,7 @@
         <v>1</v>
       </c>
       <c r="K173" t="n">
-        <v>-10.6337108291888</v>
+        <v>-10.6337108294742</v>
       </c>
       <c r="L173" t="n">
         <v>0</v>
@@ -6643,10 +6643,10 @@
         <v>0</v>
       </c>
       <c r="G174" t="n">
-        <v>0.751549114929546</v>
+        <v>0.751549114898618</v>
       </c>
       <c r="H174" t="n">
-        <v>0.10292804603507</v>
+        <v>0.102928046026131</v>
       </c>
       <c r="I174" t="e">
         <v>#NUM!</v>
@@ -6655,7 +6655,7 @@
         <v>1</v>
       </c>
       <c r="K174" t="n">
-        <v>-2.08550051743769</v>
+        <v>-2.08550051783347</v>
       </c>
       <c r="L174" t="n">
         <v>1</v>
@@ -6681,10 +6681,10 @@
         <v>0</v>
       </c>
       <c r="G175" t="n">
-        <v>0.523590581222707</v>
+        <v>0.523590581247177</v>
       </c>
       <c r="H175" t="n">
-        <v>0.0274283570549565</v>
+        <v>0.0274283570579094</v>
       </c>
       <c r="I175" t="e">
         <v>#NUM!</v>
@@ -6693,7 +6693,7 @@
         <v>1</v>
       </c>
       <c r="K175" t="n">
-        <v>-12.3516982538247</v>
+        <v>-12.35169825218</v>
       </c>
       <c r="L175" t="n">
         <v>0</v>
@@ -6747,10 +6747,10 @@
         <v>0</v>
       </c>
       <c r="G177" t="n">
-        <v>0.659511027819042</v>
+        <v>0.659511027827981</v>
       </c>
       <c r="H177" t="n">
-        <v>0.0649906209857633</v>
+        <v>0.064990620990198</v>
       </c>
       <c r="I177" t="e">
         <v>#NUM!</v>
@@ -6759,7 +6759,7 @@
         <v>1</v>
       </c>
       <c r="K177" t="n">
-        <v>-4.22408348100765</v>
+        <v>-4.22408348063912</v>
       </c>
       <c r="L177" t="n">
         <v>0.004</v>
@@ -6785,10 +6785,10 @@
         <v>0</v>
       </c>
       <c r="G178" t="n">
-        <v>0.608060001015597</v>
+        <v>0.608060000979011</v>
       </c>
       <c r="H178" t="n">
-        <v>0.0830805055718608</v>
+        <v>0.0830805055630682</v>
       </c>
       <c r="I178" t="e">
         <v>#NUM!</v>
@@ -6797,7 +6797,7 @@
         <v>1</v>
       </c>
       <c r="K178" t="n">
-        <v>-3.64103143880243</v>
+        <v>-3.64103143940906</v>
       </c>
       <c r="L178" t="n">
         <v>0.042</v>
@@ -6823,10 +6823,10 @@
         <v>0</v>
       </c>
       <c r="G179" t="n">
-        <v>0.423624328770425</v>
+        <v>0.423624328782168</v>
       </c>
       <c r="H179" t="n">
-        <v>0.0218193258912026</v>
+        <v>0.021819325893217</v>
       </c>
       <c r="I179" t="e">
         <v>#NUM!</v>
@@ -6835,7 +6835,7 @@
         <v>1</v>
       </c>
       <c r="K179" t="n">
-        <v>-16.6757866730472</v>
+        <v>-16.6757866714317</v>
       </c>
       <c r="L179" t="n">
         <v>0</v>
@@ -6861,10 +6861,10 @@
         <v>0</v>
       </c>
       <c r="G180" t="n">
-        <v>0.846811242632873</v>
+        <v>0.846811242630042</v>
       </c>
       <c r="H180" t="n">
-        <v>0.0787121193343653</v>
+        <v>0.0787121193390442</v>
       </c>
       <c r="I180" t="e">
         <v>#NUM!</v>
@@ -6873,7 +6873,7 @@
         <v>1</v>
       </c>
       <c r="K180" t="n">
-        <v>-1.788868428713</v>
+        <v>-1.78886842863665</v>
       </c>
       <c r="L180" t="n">
         <v>1</v>
@@ -6899,10 +6899,10 @@
         <v>0</v>
       </c>
       <c r="G181" t="n">
-        <v>0.808744637324751</v>
+        <v>0.808744637336272</v>
       </c>
       <c r="H181" t="n">
-        <v>0.0733911383796918</v>
+        <v>0.0733911383856612</v>
       </c>
       <c r="I181" t="e">
         <v>#NUM!</v>
@@ -6911,7 +6911,7 @@
         <v>1</v>
       </c>
       <c r="K181" t="n">
-        <v>-2.33916379021887</v>
+        <v>-2.33916378990496</v>
       </c>
       <c r="L181" t="n">
         <v>1</v>
@@ -6937,10 +6937,10 @@
         <v>0</v>
       </c>
       <c r="G182" t="n">
-        <v>1.61965644114707</v>
+        <v>1.61965644114812</v>
       </c>
       <c r="H182" t="n">
-        <v>0.148388608254908</v>
+        <v>0.148388608264936</v>
       </c>
       <c r="I182" t="e">
         <v>#NUM!</v>
@@ -6949,7 +6949,7 @@
         <v>1</v>
       </c>
       <c r="K182" t="n">
-        <v>5.26334943609088</v>
+        <v>5.26334943574572</v>
       </c>
       <c r="L182" t="n">
         <v>0</v>
@@ -6975,10 +6975,10 @@
         <v>0</v>
       </c>
       <c r="G183" t="n">
-        <v>1.01868907908853</v>
+        <v>1.01868907906924</v>
       </c>
       <c r="H183" t="n">
-        <v>0.0604950234015124</v>
+        <v>0.0604950234011614</v>
       </c>
       <c r="I183" t="e">
         <v>#NUM!</v>
@@ -6987,7 +6987,7 @@
         <v>1</v>
       </c>
       <c r="K183" t="n">
-        <v>0.311804855367701</v>
+        <v>0.311804855044724</v>
       </c>
       <c r="L183" t="n">
         <v>1</v>
@@ -7013,10 +7013,10 @@
         <v>0</v>
       </c>
       <c r="G184" t="n">
-        <v>0.685134257797156</v>
+        <v>0.685134257781836</v>
       </c>
       <c r="H184" t="n">
-        <v>0.0633586339403144</v>
+        <v>0.0633586339429511</v>
       </c>
       <c r="I184" t="e">
         <v>#NUM!</v>
@@ -7025,7 +7025,7 @@
         <v>1</v>
       </c>
       <c r="K184" t="n">
-        <v>-4.08905573628635</v>
+        <v>-4.08905573626655</v>
       </c>
       <c r="L184" t="n">
         <v>0.007</v>
@@ -7051,10 +7051,10 @@
         <v>0</v>
       </c>
       <c r="G185" t="n">
-        <v>0.654335498803891</v>
+        <v>0.654335498800768</v>
       </c>
       <c r="H185" t="n">
-        <v>0.0590610280022213</v>
+        <v>0.0590610280059785</v>
       </c>
       <c r="I185" t="e">
         <v>#NUM!</v>
@@ -7063,7 +7063,7 @@
         <v>1</v>
       </c>
       <c r="K185" t="n">
-        <v>-4.69898066486124</v>
+        <v>-4.69898066459276</v>
       </c>
       <c r="L185" t="n">
         <v>0</v>
@@ -7089,10 +7089,10 @@
         <v>0</v>
       </c>
       <c r="G186" t="n">
-        <v>0.793907242088408</v>
+        <v>0.793907242114751</v>
       </c>
       <c r="H186" t="n">
-        <v>0.0832131928513175</v>
+        <v>0.0832131928585549</v>
       </c>
       <c r="I186" t="e">
         <v>#NUM!</v>
@@ -7101,7 +7101,7 @@
         <v>1</v>
       </c>
       <c r="K186" t="n">
-        <v>-2.20187175687539</v>
+        <v>-2.20187175644037</v>
       </c>
       <c r="L186" t="n">
         <v>1</v>
@@ -7127,10 +7127,10 @@
         <v>0</v>
       </c>
       <c r="G187" t="n">
-        <v>0.765597779505446</v>
+        <v>0.765597779524966</v>
       </c>
       <c r="H187" t="n">
-        <v>0.0121167974437633</v>
+        <v>0.0121167974439606</v>
       </c>
       <c r="I187" t="e">
         <v>#NUM!</v>
@@ -7139,7 +7139,7 @@
         <v>1</v>
       </c>
       <c r="K187" t="n">
-        <v>-16.8765629973555</v>
+        <v>-16.8765629959001</v>
       </c>
       <c r="L187" t="n">
         <v>0</v>
@@ -7165,10 +7165,10 @@
         <v>0</v>
       </c>
       <c r="G188" t="n">
-        <v>1.23597854434478</v>
+        <v>1.23597854436829</v>
       </c>
       <c r="H188" t="n">
-        <v>0.0190179257093596</v>
+        <v>0.0190179257094632</v>
       </c>
       <c r="I188" t="e">
         <v>#NUM!</v>
@@ -7177,7 +7177,7 @@
         <v>1</v>
       </c>
       <c r="K188" t="n">
-        <v>13.7690159415274</v>
+        <v>13.7690159429501</v>
       </c>
       <c r="L188" t="n">
         <v>0</v>
@@ -7203,10 +7203,10 @@
         <v>0</v>
       </c>
       <c r="G189" t="n">
-        <v>0.964341599267324</v>
+        <v>0.964341599259913</v>
       </c>
       <c r="H189" t="n">
-        <v>0.100717242051771</v>
+        <v>0.100717242056498</v>
       </c>
       <c r="I189" t="e">
         <v>#NUM!</v>
@@ -7215,7 +7215,7 @@
         <v>1</v>
       </c>
       <c r="K189" t="n">
-        <v>-0.347655920942992</v>
+        <v>-0.347655920997586</v>
       </c>
       <c r="L189" t="n">
         <v>1</v>
@@ -7241,10 +7241,10 @@
         <v>0</v>
       </c>
       <c r="G190" t="n">
-        <v>0.64233092533922</v>
+        <v>0.642330925348319</v>
       </c>
       <c r="H190" t="n">
-        <v>0.0670546924226365</v>
+        <v>0.0670546924272509</v>
       </c>
       <c r="I190" t="e">
         <v>#NUM!</v>
@@ -7253,7 +7253,7 @@
         <v>1</v>
       </c>
       <c r="K190" t="n">
-        <v>-4.24025273150399</v>
+        <v>-4.24025273113657</v>
       </c>
       <c r="L190" t="n">
         <v>0.003</v>
@@ -7279,10 +7279,10 @@
         <v>0</v>
       </c>
       <c r="G191" t="n">
-        <v>0.619426431800484</v>
+        <v>0.619426431804498</v>
       </c>
       <c r="H191" t="n">
-        <v>0.00835245121817608</v>
+        <v>0.00835245121831939</v>
       </c>
       <c r="I191" t="e">
         <v>#NUM!</v>
@@ -7291,7 +7291,7 @@
         <v>1</v>
       </c>
       <c r="K191" t="n">
-        <v>-35.5202689021657</v>
+        <v>-35.5202689013059</v>
       </c>
       <c r="L191" t="n">
         <v>0</v>

</xml_diff>